<commit_message>
More updates to CiLVpUAAbP
Still incomplete, reorganization of existing data and removal of sources which did not have relevant data.
</commit_message>
<xml_diff>
--- a/InputData/land/CiLVpUAAbP/Chg in Land Val per Unit Area Affected by Pol.xlsx
+++ b/InputData/land/CiLVpUAAbP/Chg in Land Val per Unit Area Affected by Pol.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\OneDrive\Desktop\Models\eps-brazil-cpl2\InputData\land\CiLVpUAAbP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c201c4a77399164c/Desktop/Models/eps-brazil-cpl2/InputData/land/CiLVpUAAbP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D71E18-5840-40D9-B623-17FCD8C4AFB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{1CB1CDC3-E76E-47DB-938E-DED291C84E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F5E2758-B9E5-4767-AF7B-16C36D6F4F76}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="6" r:id="rId2"/>
-    <sheet name="CiLVpUAAbP" sheetId="3" r:id="rId3"/>
+    <sheet name="Highlighted Data" sheetId="7" r:id="rId3"/>
+    <sheet name="CiLVpUAAbP" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
   <definedNames>
     <definedName name="C_to_CO2">'[1]Conversion Factors'!$A$4</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>CiLVpUAAbP Change in Land Value per Unit Area Affected by Policy</t>
   </si>
@@ -118,9 +119,6 @@
     <t>Conversion to $USD2012/acre</t>
   </si>
   <si>
-    <t>Reforestation &amp; Forest Restoration</t>
-  </si>
-  <si>
     <t>Brazil Farmland Surge</t>
   </si>
   <si>
@@ -148,19 +146,61 @@
     <t>Farmland Value $USD2012/acre</t>
   </si>
   <si>
-    <t>The economic value of the Brazilian Amazon rainforest ecosystem services: A metaanalysis of the Brazilian literature</t>
-  </si>
-  <si>
-    <t>Brouwer, R., Pinto, R., Dugstad, A., &amp; Navrud, S. (2022). The economic value of the Brazilian Amazon rainforest ecosystem services: A meta-analysis of the Brazilian literature. PloS one, 17(5), e0268425.</t>
-  </si>
-  <si>
-    <t>https://doi.org/10.1371/journal.pone.0268425</t>
-  </si>
-  <si>
     <t>Farmland $USD/ha</t>
   </si>
   <si>
     <t>Reforestation</t>
+  </si>
+  <si>
+    <t>Farmland Prices in Brazil More than Doubled in the Last Three Years</t>
+  </si>
+  <si>
+    <t>Colussi, J., Schnitkey, G., Paulson, N., &amp; Baltz, J. (2023). Farmland Prices in Brazil More than Doubled in the Last Three Years. farmdoc daily, 13(79).</t>
+  </si>
+  <si>
+    <t>https://farmdocdaily.illinois.edu/2023/04/farmland-prices-in-brazil-more-than-doubled-in-the-last-three-years.html</t>
+  </si>
+  <si>
+    <t>&lt;- Potentially better data as first reforestation source</t>
+  </si>
+  <si>
+    <t>Forest Set Aside</t>
+  </si>
+  <si>
+    <t>The value of property rights and environmental policy in Brazil: Evidence from a new database on land prices</t>
+  </si>
+  <si>
+    <t>Moffette, F., Phaneuf, D., Rausch, L., &amp; Gibbs, H. K. (2024). The value of property rights and environmental policy in Brazil: Evidence from a new database on land prices. Global Environmental Change, 87, 102854.</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.gloenvcha.2024.102854</t>
+  </si>
+  <si>
+    <t>&lt;- Contains tables with the land data and prices but does not elaborate on their change over time.</t>
+  </si>
+  <si>
+    <t>Could also potentially apply to forest restoration.</t>
+  </si>
+  <si>
+    <t>Cropland Value</t>
+  </si>
+  <si>
+    <t>Cropland Value/acre</t>
+  </si>
+  <si>
+    <t>$USD 2012/2022</t>
+  </si>
+  <si>
+    <t>Planted Forest/acre</t>
+  </si>
+  <si>
+    <t>Planted Forest</t>
+  </si>
+  <si>
+    <t>Change in Value</t>
+  </si>
+  <si>
+    <t>Might be worth contacting them to see if they would have the data we want, but it is not in the report.</t>
   </si>
 </sst>
 </file>
@@ -226,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +276,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -305,7 +351,7 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -317,10 +363,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Body: normal cell" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -689,11 +736,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -701,12 +746,12 @@
     <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -714,129 +759,169 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>2024</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B15" s="9" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B14" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B15" s="11" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B16" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B20" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B21" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A28" s="1" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B29">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B38">
         <v>6.0757389000000002</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C38" t="s">
         <v>20</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D38" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B30">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B39">
         <v>2.4710538149999999</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C39" t="s">
         <v>22</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B31">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B40">
         <v>247.10538149999999</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B41" s="7">
+        <v>1.05</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B42" s="7">
+        <v>0.89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B43" s="7">
+        <v>0.78</v>
+      </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B44" s="7">
+        <v>0.75</v>
+      </c>
+      <c r="C44" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B32" s="7">
-        <v>1.05</v>
-      </c>
-      <c r="C32" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B33" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
-      <c r="B34" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="C34" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -872,12 +957,12 @@
         <v>2023</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2">
         <v>2023</v>
@@ -908,7 +993,7 @@
         <v>2093</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G4">
         <v>11000</v>
@@ -935,26 +1020,26 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="7">
-        <f>D5*About!B29*About!B32</f>
+        <f>D5*About!B38*About!B41</f>
         <v>1913.8577535000002</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="7">
-        <f>G4*About!B34/About!B30</f>
+        <f>G4*About!B44/About!B39</f>
         <v>3338.6565480363688</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="8">
-        <f>B10/(D4*About!B31)</f>
+        <f>B10/(D4*About!B40)</f>
         <v>3.7004813857058594E-3</v>
       </c>
       <c r="G11" s="7"/>
@@ -968,6 +1053,101 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F214405-0DDE-40EE-B2F7-FFED58ECB09E}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B3">
+        <v>2019</v>
+      </c>
+      <c r="C3">
+        <v>2021</v>
+      </c>
+      <c r="D3">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4">
+        <v>1875</v>
+      </c>
+      <c r="C4">
+        <v>2941</v>
+      </c>
+      <c r="D4">
+        <v>4721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5">
+        <v>938</v>
+      </c>
+      <c r="C5">
+        <v>994</v>
+      </c>
+      <c r="D5">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="7">
+        <f>D4*About!B43</f>
+        <v>3682.38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="7">
+        <f>D5*About!B43</f>
+        <v>1124.76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="7">
+        <f>D10-D11</f>
+        <v>2557.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
@@ -975,7 +1155,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1017,7 +1197,7 @@
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <f>Data!B11</f>
         <v>3.7004813857058594E-3</v>
       </c>

</xml_diff>